<commit_message>
Stashing changes for merge
</commit_message>
<xml_diff>
--- a/Year1_FoCS_Timetable.xlsx
+++ b/Year1_FoCS_Timetable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://qubstudentcloud-my.sharepoint.com/personal/3057234_ads_qub_ac_uk/Documents/Documents/timetable_web_application-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="8_{B9763A23-CB07-42C7-A995-D64E6EF74790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB210CC4-3467-4A29-AEE6-E55228A2FFAB}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="8_{B9763A23-CB07-42C7-A995-D64E6EF74790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BC42946-2F4E-4709-AFE8-DF295E5C1A84}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="24WkTimetable" sheetId="1" r:id="rId1"/>
@@ -2295,6 +2295,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2558,13 +2562,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P7973"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A476" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I506" sqref="I506"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J510" sqref="J510"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2633,7 +2637,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -2681,7 +2685,7 @@
         <v>45187</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -2727,7 +2731,7 @@
         <v>45188</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -2773,7 +2777,7 @@
         <v>45189</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2819,7 +2823,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -2865,7 +2869,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -2911,7 +2915,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -2957,7 +2961,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3003,7 +3007,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -3049,7 +3053,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" s="1" customFormat="1" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -3095,7 +3099,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" s="1" customFormat="1" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -3141,7 +3145,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -3187,7 +3191,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -3233,7 +3237,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -3279,7 +3283,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -3325,7 +3329,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -3371,7 +3375,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -3417,7 +3421,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -3463,7 +3467,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -3509,7 +3513,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -3555,7 +3559,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -3601,7 +3605,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
@@ -3647,7 +3651,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
@@ -3693,7 +3697,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -3739,7 +3743,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -3785,7 +3789,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>14</v>
       </c>
@@ -3831,7 +3835,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
@@ -3877,7 +3881,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -3923,7 +3927,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
@@ -3969,7 +3973,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" s="1" customFormat="1" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
@@ -4015,7 +4019,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" s="1" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
@@ -4061,7 +4065,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" s="1" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
@@ -4107,7 +4111,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="1" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" s="1" customFormat="1" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
@@ -4153,7 +4157,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="1" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" s="1" customFormat="1" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>14</v>
       </c>
@@ -4199,7 +4203,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="1" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" s="1" customFormat="1" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
@@ -4245,7 +4249,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" s="1" customFormat="1" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
@@ -4293,7 +4297,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" s="1" customFormat="1" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>14</v>
       </c>
@@ -4341,7 +4345,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" s="1" customFormat="1" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>14</v>
       </c>
@@ -4389,7 +4393,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" s="1" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>14</v>
       </c>
@@ -4435,7 +4439,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" s="1" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>14</v>
       </c>
@@ -4481,7 +4485,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" s="1" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>14</v>
       </c>
@@ -4527,7 +4531,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" s="1" customFormat="1" ht="16.149999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>14</v>
       </c>
@@ -4573,7 +4577,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="1" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" s="1" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>14</v>
       </c>
@@ -4619,7 +4623,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" s="1" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>14</v>
       </c>
@@ -4665,7 +4669,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="1" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" s="1" customFormat="1" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -4711,7 +4715,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" s="1" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>14</v>
       </c>
@@ -4757,7 +4761,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="1" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" s="1" customFormat="1" ht="18.600000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>14</v>
       </c>
@@ -4805,7 +4809,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" s="1" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
@@ -4853,7 +4857,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="1" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" s="1" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>14</v>
       </c>
@@ -4899,7 +4903,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" s="1" customFormat="1" ht="15.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>14</v>
       </c>
@@ -4945,7 +4949,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" s="1" customFormat="1" ht="16.149999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>14</v>
       </c>
@@ -4991,7 +4995,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" s="1" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>14</v>
       </c>
@@ -5037,7 +5041,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" s="1" customFormat="1" ht="11.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>14</v>
       </c>
@@ -5083,7 +5087,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>14</v>
       </c>
@@ -5129,7 +5133,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" s="1" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>14</v>
       </c>
@@ -5177,7 +5181,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" s="1" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>14</v>
       </c>
@@ -5225,7 +5229,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="58" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>14</v>
       </c>
@@ -5271,7 +5275,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="59" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>14</v>
       </c>
@@ -5317,7 +5321,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="60" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>14</v>
       </c>
@@ -5363,7 +5367,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="61" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>14</v>
       </c>
@@ -5409,7 +5413,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="62" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" s="1" customFormat="1" ht="11.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>14</v>
       </c>
@@ -5455,7 +5459,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="63" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" s="1" customFormat="1" ht="11.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>14</v>
       </c>
@@ -5501,7 +5505,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="64" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" s="1" customFormat="1" ht="11.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>14</v>
       </c>
@@ -5547,7 +5551,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>14</v>
       </c>
@@ -5593,7 +5597,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="1" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" s="1" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>14</v>
       </c>
@@ -5639,7 +5643,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="1" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" s="1" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>14</v>
       </c>
@@ -5685,7 +5689,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="1" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" s="1" customFormat="1" ht="14.65" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>14</v>
       </c>
@@ -5731,7 +5735,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="1" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" s="1" customFormat="1" ht="16.149999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>14</v>
       </c>
@@ -5777,7 +5781,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="70" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" s="1" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>14</v>
       </c>
@@ -5825,7 +5829,7 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="71" spans="1:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" s="1" customFormat="1" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>14</v>
       </c>
@@ -5873,7 +5877,7 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="72" spans="1:16" s="1" customFormat="1" ht="34.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" s="1" customFormat="1" ht="34.15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>14</v>
       </c>
@@ -5921,7 +5925,7 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" s="1" customFormat="1" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>14</v>
       </c>
@@ -5969,7 +5973,7 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" s="1" customFormat="1" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>14</v>
       </c>
@@ -6017,7 +6021,7 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="75" spans="1:16" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" s="1" customFormat="1" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>14</v>
       </c>
@@ -6065,7 +6069,7 @@
         <v>45196</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" s="1" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>14</v>
       </c>
@@ -6113,7 +6117,7 @@
         <v>45196</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>14</v>
       </c>
@@ -6161,7 +6165,7 @@
         <v>45196</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" s="1" customFormat="1" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>14</v>
       </c>
@@ -6209,7 +6213,7 @@
         <v>45196</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" s="1" customFormat="1" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>14</v>
       </c>
@@ -6257,7 +6261,7 @@
         <v>45196</v>
       </c>
     </row>
-    <row r="80" spans="1:16" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" s="1" customFormat="1" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>14</v>
       </c>
@@ -6305,7 +6309,7 @@
         <v>45196</v>
       </c>
     </row>
-    <row r="81" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>14</v>
       </c>
@@ -6353,7 +6357,7 @@
         <v>45196</v>
       </c>
     </row>
-    <row r="82" spans="1:16" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" s="1" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>14</v>
       </c>
@@ -6401,7 +6405,7 @@
         <v>45196</v>
       </c>
     </row>
-    <row r="83" spans="1:16" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" s="1" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>14</v>
       </c>
@@ -6447,7 +6451,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="84" spans="1:16" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" s="1" customFormat="1" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>14</v>
       </c>
@@ -6493,7 +6497,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="85" spans="1:16" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" s="1" customFormat="1" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>14</v>
       </c>
@@ -6539,7 +6543,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="86" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" s="1" customFormat="1" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>14</v>
       </c>
@@ -6585,7 +6589,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="87" spans="1:16" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" s="1" customFormat="1" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>14</v>
       </c>
@@ -6631,7 +6635,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="88" spans="1:16" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" s="1" customFormat="1" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>14</v>
       </c>
@@ -6677,7 +6681,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="89" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>14</v>
       </c>
@@ -6723,7 +6727,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="90" spans="1:16" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" s="1" customFormat="1" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>14</v>
       </c>
@@ -6769,7 +6773,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="91" spans="1:16" s="1" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" s="1" customFormat="1" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>14</v>
       </c>
@@ -6815,7 +6819,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="92" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>14</v>
       </c>
@@ -6861,7 +6865,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="93" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>14</v>
       </c>
@@ -6907,7 +6911,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="94" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>14</v>
       </c>
@@ -6953,7 +6957,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="95" spans="1:16" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" s="1" customFormat="1" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>14</v>
       </c>
@@ -6999,7 +7003,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="96" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>14</v>
       </c>
@@ -7045,7 +7049,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="97" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>14</v>
       </c>
@@ -7091,7 +7095,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="98" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>14</v>
       </c>
@@ -7137,7 +7141,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="99" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>14</v>
       </c>
@@ -7183,7 +7187,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="100" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>14</v>
       </c>
@@ -7229,7 +7233,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="101" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>14</v>
       </c>
@@ -7277,7 +7281,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="102" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>14</v>
       </c>
@@ -7323,7 +7327,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="103" spans="1:16" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" s="1" customFormat="1" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>14</v>
       </c>
@@ -7369,7 +7373,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="104" spans="1:16" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" s="1" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>14</v>
       </c>
@@ -7415,7 +7419,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="105" spans="1:16" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" s="1" customFormat="1" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>14</v>
       </c>
@@ -7461,7 +7465,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="106" spans="1:16" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" s="1" customFormat="1" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>14</v>
       </c>
@@ -7507,7 +7511,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="107" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>14</v>
       </c>
@@ -7553,7 +7557,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="108" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16" s="1" customFormat="1" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>14</v>
       </c>
@@ -7601,7 +7605,7 @@
         <v>45197</v>
       </c>
     </row>
-    <row r="109" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>14</v>
       </c>
@@ -7649,7 +7653,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="110" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>14</v>
       </c>
@@ -7697,7 +7701,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="111" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>14</v>
       </c>
@@ -7745,7 +7749,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="112" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="106" t="s">
         <v>14</v>
       </c>
@@ -7793,7 +7797,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="113" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>14</v>
       </c>
@@ -7841,7 +7845,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="114" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>14</v>
       </c>
@@ -7889,7 +7893,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="115" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>14</v>
       </c>
@@ -7937,7 +7941,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="116" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>14</v>
       </c>
@@ -7985,7 +7989,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="117" spans="1:16" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" s="1" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>14</v>
       </c>
@@ -8033,7 +8037,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="118" spans="1:16" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" s="1" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>14</v>
       </c>
@@ -8081,7 +8085,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="119" spans="1:16" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" s="1" customFormat="1" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>14</v>
       </c>
@@ -8129,7 +8133,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="120" spans="1:16" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" s="1" customFormat="1" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>14</v>
       </c>
@@ -8177,7 +8181,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="121" spans="1:16" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" s="1" customFormat="1" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>14</v>
       </c>
@@ -8225,7 +8229,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="122" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>14</v>
       </c>
@@ -8273,7 +8277,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="123" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>14</v>
       </c>
@@ -8321,7 +8325,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="124" spans="1:16" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" s="1" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>14</v>
       </c>
@@ -8369,7 +8373,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="125" spans="1:16" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" s="1" customFormat="1" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>14</v>
       </c>
@@ -8417,7 +8421,7 @@
         <v>45201</v>
       </c>
     </row>
-    <row r="126" spans="1:16" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" s="1" customFormat="1" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>14</v>
       </c>
@@ -8465,7 +8469,7 @@
         <v>45201</v>
       </c>
     </row>
-    <row r="127" spans="1:16" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" s="1" customFormat="1" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>14</v>
       </c>
@@ -8513,7 +8517,7 @@
         <v>45201</v>
       </c>
     </row>
-    <row r="128" spans="1:16" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" s="1" customFormat="1" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>14</v>
       </c>
@@ -8561,7 +8565,7 @@
         <v>45201</v>
       </c>
     </row>
-    <row r="129" spans="1:16" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" s="1" customFormat="1" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>14</v>
       </c>
@@ -8609,7 +8613,7 @@
         <v>45201</v>
       </c>
     </row>
-    <row r="130" spans="1:16" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" s="1" customFormat="1" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>14</v>
       </c>
@@ -8657,7 +8661,7 @@
         <v>45201</v>
       </c>
     </row>
-    <row r="131" spans="1:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" s="1" customFormat="1" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>14</v>
       </c>
@@ -8705,7 +8709,7 @@
         <v>45201</v>
       </c>
     </row>
-    <row r="132" spans="1:16" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" s="1" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>14</v>
       </c>
@@ -8753,7 +8757,7 @@
         <v>45201</v>
       </c>
     </row>
-    <row r="133" spans="1:16" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" s="1" customFormat="1" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>14</v>
       </c>
@@ -8799,7 +8803,7 @@
         <v>45201</v>
       </c>
     </row>
-    <row r="134" spans="1:16" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" s="1" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>14</v>
       </c>
@@ -8845,7 +8849,7 @@
         <v>45201</v>
       </c>
     </row>
-    <row r="135" spans="1:16" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16" s="1" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>14</v>
       </c>
@@ -8893,7 +8897,7 @@
         <v>45201</v>
       </c>
     </row>
-    <row r="136" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>14</v>
       </c>
@@ -8941,7 +8945,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="137" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>14</v>
       </c>
@@ -8989,7 +8993,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="138" spans="1:16" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" s="1" customFormat="1" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>14</v>
       </c>
@@ -9035,7 +9039,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="139" spans="1:16" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" s="1" customFormat="1" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>14</v>
       </c>
@@ -9083,7 +9087,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="140" spans="1:16" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16" s="1" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>14</v>
       </c>
@@ -9131,7 +9135,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="141" spans="1:16" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16" s="1" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>14</v>
       </c>
@@ -9179,7 +9183,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="142" spans="1:16" s="1" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" s="1" customFormat="1" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>14</v>
       </c>
@@ -9227,7 +9231,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="143" spans="1:16" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" s="1" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>14</v>
       </c>
@@ -9275,7 +9279,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="144" spans="1:16" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16" s="1" customFormat="1" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>14</v>
       </c>
@@ -9323,7 +9327,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="145" spans="1:16" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16" s="1" customFormat="1" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>14</v>
       </c>
@@ -9371,7 +9375,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="146" spans="1:16" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" s="1" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>14</v>
       </c>
@@ -9419,7 +9423,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="147" spans="1:16" s="1" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:16" s="1" customFormat="1" ht="19.149999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>14</v>
       </c>
@@ -9467,7 +9471,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="148" spans="1:16" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:16" s="1" customFormat="1" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>14</v>
       </c>
@@ -9515,7 +9519,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="149" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>14</v>
       </c>
@@ -9563,7 +9567,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="150" spans="1:16" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:16" s="1" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>14</v>
       </c>
@@ -9611,7 +9615,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="151" spans="1:16" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:16" s="1" customFormat="1" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>14</v>
       </c>
@@ -9659,7 +9663,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="152" spans="1:16" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:16" s="1" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>14</v>
       </c>
@@ -9707,7 +9711,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="153" spans="1:16" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:16" s="1" customFormat="1" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>14</v>
       </c>
@@ -9755,7 +9759,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="154" spans="1:16" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:16" s="1" customFormat="1" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>14</v>
       </c>
@@ -9803,7 +9807,7 @@
         <v>45203</v>
       </c>
     </row>
-    <row r="155" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>14</v>
       </c>
@@ -9849,7 +9853,7 @@
         <v>45204</v>
       </c>
     </row>
-    <row r="156" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>14</v>
       </c>
@@ -9895,7 +9899,7 @@
         <v>45204</v>
       </c>
     </row>
-    <row r="157" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:16" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>14</v>
       </c>
@@ -9943,7 +9947,7 @@
         <v>45204</v>
       </c>
     </row>
-    <row r="158" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:16" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>14</v>
       </c>
@@ -9991,7 +9995,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="159" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:16" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>14</v>
       </c>
@@ -10039,7 +10043,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="160" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:16" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>14</v>
       </c>
@@ -10087,7 +10091,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="161" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:16" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>14</v>
       </c>
@@ -10135,7 +10139,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="162" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:16" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>14</v>
       </c>
@@ -10183,7 +10187,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="163" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:16" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>14</v>
       </c>
@@ -10231,7 +10235,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="164" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>14</v>
       </c>
@@ -10279,7 +10283,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="165" spans="1:16" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:16" s="1" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>14</v>
       </c>
@@ -10327,7 +10331,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="166" spans="1:16" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:16" s="1" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>14</v>
       </c>
@@ -10375,7 +10379,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="167" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:16" s="1" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>14</v>
       </c>
@@ -10423,7 +10427,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="168" spans="1:16" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:16" s="1" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>14</v>
       </c>
@@ -10471,7 +10475,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="169" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>14</v>
       </c>
@@ -10519,7 +10523,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="170" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>14</v>
       </c>
@@ -10567,7 +10571,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="171" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>14</v>
       </c>
@@ -10615,7 +10619,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="172" spans="1:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:16" s="1" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>14</v>
       </c>
@@ -10663,7 +10667,7 @@
         <v>45205</v>
       </c>
     </row>
-    <row r="173" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:16" s="1" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>14</v>
       </c>
@@ -10711,7 +10715,7 @@
         <v>45208</v>
       </c>
     </row>
-    <row r="174" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:16" s="1" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>14</v>
       </c>
@@ -10759,7 +10763,7 @@
         <v>45208</v>
       </c>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>14</v>
       </c>
@@ -10807,7 +10811,7 @@
         <v>45208</v>
       </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>14</v>
       </c>
@@ -10855,7 +10859,7 @@
         <v>45208</v>
       </c>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>14</v>
       </c>
@@ -10901,7 +10905,7 @@
         <v>45208</v>
       </c>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>14</v>
       </c>
@@ -10947,7 +10951,7 @@
         <v>45208</v>
       </c>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>14</v>
       </c>
@@ -10993,7 +10997,7 @@
         <v>45208</v>
       </c>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>14</v>
       </c>
@@ -11039,7 +11043,7 @@
         <v>45208</v>
       </c>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>14</v>
       </c>
@@ -11087,7 +11091,7 @@
         <v>45209</v>
       </c>
     </row>
-    <row r="182" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>14</v>
       </c>
@@ -11135,7 +11139,7 @@
         <v>45209</v>
       </c>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>14</v>
       </c>
@@ -11183,7 +11187,7 @@
         <v>45209</v>
       </c>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>14</v>
       </c>
@@ -11229,7 +11233,7 @@
         <v>45209</v>
       </c>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>14</v>
       </c>
@@ -11275,7 +11279,7 @@
         <v>45209</v>
       </c>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>14</v>
       </c>
@@ -11321,7 +11325,7 @@
         <v>45209</v>
       </c>
     </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>14</v>
       </c>
@@ -11367,7 +11371,7 @@
         <v>45209</v>
       </c>
     </row>
-    <row r="188" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>14</v>
       </c>
@@ -11415,7 +11419,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="189" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>14</v>
       </c>
@@ -11463,7 +11467,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>14</v>
       </c>
@@ -11511,7 +11515,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="191" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>14</v>
       </c>
@@ -11559,7 +11563,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="192" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>14</v>
       </c>
@@ -11607,7 +11611,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="193" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>14</v>
       </c>
@@ -11655,7 +11659,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="194" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>14</v>
       </c>
@@ -11703,7 +11707,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="195" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>14</v>
       </c>
@@ -11751,7 +11755,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="196" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>14</v>
       </c>
@@ -11799,7 +11803,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>14</v>
       </c>
@@ -11847,7 +11851,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="198" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>14</v>
       </c>
@@ -11895,7 +11899,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="199" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>14</v>
       </c>
@@ -11943,7 +11947,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="200" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>14</v>
       </c>
@@ -11991,7 +11995,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="201" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>14</v>
       </c>
@@ -12039,7 +12043,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>14</v>
       </c>
@@ -12087,7 +12091,7 @@
         <v>45211</v>
       </c>
     </row>
-    <row r="203" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>14</v>
       </c>
@@ -12135,7 +12139,7 @@
         <v>45211</v>
       </c>
     </row>
-    <row r="204" spans="1:16" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:16" ht="23.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>14</v>
       </c>
@@ -12183,7 +12187,7 @@
         <v>45211</v>
       </c>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>14</v>
       </c>
@@ -12231,7 +12235,7 @@
         <v>45211</v>
       </c>
     </row>
-    <row r="206" spans="1:16" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:16" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>14</v>
       </c>
@@ -12279,7 +12283,7 @@
         <v>45211</v>
       </c>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>14</v>
       </c>
@@ -12327,7 +12331,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>14</v>
       </c>
@@ -12375,7 +12379,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>14</v>
       </c>
@@ -12423,7 +12427,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="210" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:16" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>14</v>
       </c>
@@ -12471,7 +12475,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="211" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:16" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>14</v>
       </c>
@@ -12519,7 +12523,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="212" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:16" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>14</v>
       </c>
@@ -12567,7 +12571,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="213" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:16" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>14</v>
       </c>
@@ -12615,7 +12619,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="214" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:16" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>14</v>
       </c>
@@ -12663,7 +12667,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>14</v>
       </c>
@@ -12711,7 +12715,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="216" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>14</v>
       </c>
@@ -12759,7 +12763,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>14</v>
       </c>
@@ -12807,7 +12811,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>14</v>
       </c>
@@ -12855,7 +12859,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>14</v>
       </c>
@@ -12903,7 +12907,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>14</v>
       </c>
@@ -12951,7 +12955,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>14</v>
       </c>
@@ -12999,7 +13003,7 @@
         <v>45212</v>
       </c>
     </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>14</v>
       </c>
@@ -13045,7 +13049,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>14</v>
       </c>
@@ -13091,7 +13095,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>14</v>
       </c>
@@ -13137,7 +13141,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>14</v>
       </c>
@@ -13183,7 +13187,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="226" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>14</v>
       </c>
@@ -13229,7 +13233,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>14</v>
       </c>
@@ -13275,7 +13279,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>14</v>
       </c>
@@ -13323,7 +13327,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>14</v>
       </c>
@@ -13371,7 +13375,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>14</v>
       </c>
@@ -13419,7 +13423,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>14</v>
       </c>
@@ -13467,7 +13471,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>14</v>
       </c>
@@ -13513,7 +13517,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="233" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>14</v>
       </c>
@@ -13559,7 +13563,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>14</v>
       </c>
@@ -13605,7 +13609,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>14</v>
       </c>
@@ -13651,7 +13655,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>14</v>
       </c>
@@ -13697,7 +13701,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>14</v>
       </c>
@@ -13743,7 +13747,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>14</v>
       </c>
@@ -13791,7 +13795,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>14</v>
       </c>
@@ -13839,7 +13843,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>14</v>
       </c>
@@ -13887,7 +13891,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>14</v>
       </c>
@@ -13935,7 +13939,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>14</v>
       </c>
@@ -13981,7 +13985,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="243" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>14</v>
       </c>
@@ -14027,7 +14031,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="244" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>14</v>
       </c>
@@ -14073,7 +14077,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>14</v>
       </c>
@@ -14119,7 +14123,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="246" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>14</v>
       </c>
@@ -14165,7 +14169,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="247" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>14</v>
       </c>
@@ -14211,7 +14215,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>14</v>
       </c>
@@ -14259,7 +14263,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>14</v>
       </c>
@@ -14305,7 +14309,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>14</v>
       </c>
@@ -14351,7 +14355,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>14</v>
       </c>
@@ -14397,7 +14401,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>14</v>
       </c>
@@ -14443,7 +14447,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="253" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:16" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>14</v>
       </c>
@@ -14489,7 +14493,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="254" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:16" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>14</v>
       </c>
@@ -14535,7 +14539,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="255" spans="1:16" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:16" ht="25.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>14</v>
       </c>
@@ -14583,7 +14587,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="256" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:16" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>14</v>
       </c>
@@ -14631,7 +14635,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="257" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:16" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>14</v>
       </c>
@@ -14679,7 +14683,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="258" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>14</v>
       </c>
@@ -14727,7 +14731,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>14</v>
       </c>
@@ -14775,7 +14779,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="260" spans="1:16" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:16" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>14</v>
       </c>
@@ -14823,7 +14827,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="261" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>14</v>
       </c>
@@ -14871,7 +14875,7 @@
         <v>45217</v>
       </c>
     </row>
-    <row r="262" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>14</v>
       </c>
@@ -14919,7 +14923,7 @@
         <v>45217</v>
       </c>
     </row>
-    <row r="263" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>14</v>
       </c>
@@ -14967,7 +14971,7 @@
         <v>45217</v>
       </c>
     </row>
-    <row r="264" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>14</v>
       </c>
@@ -15015,7 +15019,7 @@
         <v>45217</v>
       </c>
     </row>
-    <row r="265" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>14</v>
       </c>
@@ -15063,7 +15067,7 @@
         <v>45217</v>
       </c>
     </row>
-    <row r="266" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>14</v>
       </c>
@@ -15111,7 +15115,7 @@
         <v>45217</v>
       </c>
     </row>
-    <row r="267" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>14</v>
       </c>
@@ -15159,7 +15163,7 @@
         <v>45217</v>
       </c>
     </row>
-    <row r="268" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>14</v>
       </c>
@@ -15207,7 +15211,7 @@
         <v>45217</v>
       </c>
     </row>
-    <row r="269" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>14</v>
       </c>
@@ -15255,7 +15259,7 @@
         <v>45217</v>
       </c>
     </row>
-    <row r="270" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>14</v>
       </c>
@@ -15303,7 +15307,7 @@
         <v>45217</v>
       </c>
     </row>
-    <row r="271" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>14</v>
       </c>
@@ -15351,7 +15355,7 @@
         <v>45217</v>
       </c>
     </row>
-    <row r="272" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>14</v>
       </c>
@@ -15399,7 +15403,7 @@
         <v>45217</v>
       </c>
     </row>
-    <row r="273" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>14</v>
       </c>
@@ -15447,7 +15451,7 @@
         <v>45217</v>
       </c>
     </row>
-    <row r="274" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>14</v>
       </c>
@@ -15495,7 +15499,7 @@
         <v>45217</v>
       </c>
     </row>
-    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>14</v>
       </c>
@@ -15541,7 +15545,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>14</v>
       </c>
@@ -15587,7 +15591,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="277" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>14</v>
       </c>
@@ -15633,7 +15637,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>14</v>
       </c>
@@ -15679,7 +15683,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="279" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>14</v>
       </c>
@@ -15725,7 +15729,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="280" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>14</v>
       </c>
@@ -15771,7 +15775,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="281" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>14</v>
       </c>
@@ -15817,7 +15821,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="282" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>14</v>
       </c>
@@ -15863,7 +15867,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="283" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>14</v>
       </c>
@@ -15909,7 +15913,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="284" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>14</v>
       </c>
@@ -15955,7 +15959,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>14</v>
       </c>
@@ -16001,7 +16005,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>14</v>
       </c>
@@ -16047,7 +16051,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>14</v>
       </c>
@@ -16093,7 +16097,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>14</v>
       </c>
@@ -16139,7 +16143,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="289" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>14</v>
       </c>
@@ -16185,7 +16189,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="290" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>14</v>
       </c>
@@ -16231,7 +16235,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="291" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>14</v>
       </c>
@@ -16277,7 +16281,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="292" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
         <v>14</v>
       </c>
@@ -16323,7 +16327,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="293" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>14</v>
       </c>
@@ -16369,7 +16373,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="294" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>14</v>
       </c>
@@ -16415,7 +16419,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="295" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>14</v>
       </c>
@@ -16461,7 +16465,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="296" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>14</v>
       </c>
@@ -16507,7 +16511,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="297" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>14</v>
       </c>
@@ -16553,7 +16557,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="298" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>14</v>
       </c>
@@ -16599,7 +16603,7 @@
         <v>45218</v>
       </c>
     </row>
-    <row r="299" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>14</v>
       </c>
@@ -16647,7 +16651,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="300" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>14</v>
       </c>
@@ -16695,7 +16699,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="301" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
         <v>14</v>
       </c>
@@ -16743,7 +16747,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="302" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
         <v>14</v>
       </c>
@@ -16791,7 +16795,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="303" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
         <v>14</v>
       </c>
@@ -16839,7 +16843,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="304" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
         <v>14</v>
       </c>
@@ -16887,7 +16891,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="305" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
         <v>14</v>
       </c>
@@ -16935,7 +16939,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="306" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
         <v>14</v>
       </c>
@@ -16983,7 +16987,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="307" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
         <v>14</v>
       </c>
@@ -17031,7 +17035,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="308" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
         <v>14</v>
       </c>
@@ -17079,7 +17083,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="309" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
         <v>14</v>
       </c>
@@ -17127,7 +17131,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="310" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
         <v>14</v>
       </c>
@@ -17175,7 +17179,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="311" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
         <v>14</v>
       </c>
@@ -17223,7 +17227,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="312" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
         <v>14</v>
       </c>
@@ -17271,7 +17275,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="313" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
         <v>14</v>
       </c>
@@ -17319,7 +17323,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="314" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
         <v>14</v>
       </c>
@@ -17367,7 +17371,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="315" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
         <v>14</v>
       </c>
@@ -17415,7 +17419,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="316" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
         <v>14</v>
       </c>
@@ -17463,7 +17467,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="317" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
         <v>14</v>
       </c>
@@ -17511,7 +17515,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="318" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
         <v>14</v>
       </c>
@@ -17559,7 +17563,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="319" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
         <v>14</v>
       </c>
@@ -17607,7 +17611,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="320" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
         <v>14</v>
       </c>
@@ -17655,7 +17659,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="321" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
         <v>14</v>
       </c>
@@ -17703,7 +17707,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="322" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
         <v>14</v>
       </c>
@@ -17751,7 +17755,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="323" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
         <v>14</v>
       </c>
@@ -17799,7 +17803,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="324" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
         <v>14</v>
       </c>
@@ -17847,7 +17851,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="325" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>14</v>
       </c>
@@ -17895,7 +17899,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="326" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
         <v>14</v>
       </c>
@@ -17943,7 +17947,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="327" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
         <v>14</v>
       </c>
@@ -17991,7 +17995,7 @@
         <v>45223</v>
       </c>
     </row>
-    <row r="328" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
         <v>14</v>
       </c>
@@ -18039,7 +18043,7 @@
         <v>45223</v>
       </c>
     </row>
-    <row r="329" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
         <v>14</v>
       </c>
@@ -18087,7 +18091,7 @@
         <v>45223</v>
       </c>
     </row>
-    <row r="330" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
         <v>14</v>
       </c>
@@ -18135,7 +18139,7 @@
         <v>45223</v>
       </c>
     </row>
-    <row r="331" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
         <v>14</v>
       </c>
@@ -18183,7 +18187,7 @@
         <v>45223</v>
       </c>
     </row>
-    <row r="332" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
         <v>14</v>
       </c>
@@ -18231,7 +18235,7 @@
         <v>45224</v>
       </c>
     </row>
-    <row r="333" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
         <v>14</v>
       </c>
@@ -18279,7 +18283,7 @@
         <v>45224</v>
       </c>
     </row>
-    <row r="334" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
         <v>14</v>
       </c>
@@ -18327,7 +18331,7 @@
         <v>45224</v>
       </c>
     </row>
-    <row r="335" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
         <v>14</v>
       </c>
@@ -18375,7 +18379,7 @@
         <v>45224</v>
       </c>
     </row>
-    <row r="336" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
         <v>14</v>
       </c>
@@ -18423,7 +18427,7 @@
         <v>45224</v>
       </c>
     </row>
-    <row r="337" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
         <v>14</v>
       </c>
@@ -18471,7 +18475,7 @@
         <v>45224</v>
       </c>
     </row>
-    <row r="338" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
         <v>14</v>
       </c>
@@ -18519,7 +18523,7 @@
         <v>45224</v>
       </c>
     </row>
-    <row r="339" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
         <v>14</v>
       </c>
@@ -18567,7 +18571,7 @@
         <v>45224</v>
       </c>
     </row>
-    <row r="340" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
         <v>14</v>
       </c>
@@ -18615,7 +18619,7 @@
         <v>45224</v>
       </c>
     </row>
-    <row r="341" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
         <v>14</v>
       </c>
@@ -18663,7 +18667,7 @@
         <v>45224</v>
       </c>
     </row>
-    <row r="342" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
         <v>14</v>
       </c>
@@ -18709,7 +18713,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="343" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
         <v>14</v>
       </c>
@@ -18755,7 +18759,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="344" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
         <v>14</v>
       </c>
@@ -18801,7 +18805,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="345" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
         <v>14</v>
       </c>
@@ -18847,7 +18851,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="346" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
         <v>14</v>
       </c>
@@ -18893,7 +18897,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="347" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
         <v>14</v>
       </c>
@@ -18939,7 +18943,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="348" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
         <v>14</v>
       </c>
@@ -18985,7 +18989,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="349" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
         <v>14</v>
       </c>
@@ -19031,7 +19035,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="350" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
         <v>14</v>
       </c>
@@ -19077,7 +19081,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="351" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
         <v>14</v>
       </c>
@@ -19123,7 +19127,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="352" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
         <v>14</v>
       </c>
@@ -19169,7 +19173,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="353" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
         <v>14</v>
       </c>
@@ -19215,7 +19219,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="354" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
         <v>14</v>
       </c>
@@ -19261,7 +19265,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="355" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
         <v>14</v>
       </c>
@@ -19307,7 +19311,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="356" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
         <v>14</v>
       </c>
@@ -19353,7 +19357,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="357" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
         <v>14</v>
       </c>
@@ -19399,7 +19403,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="358" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
         <v>14</v>
       </c>
@@ -19445,7 +19449,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="359" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
         <v>14</v>
       </c>
@@ -19491,7 +19495,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="360" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:16" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
         <v>14</v>
       </c>
@@ -19537,7 +19541,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="361" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:16" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
         <v>14</v>
       </c>
@@ -19583,7 +19587,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="362" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:16" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
         <v>14</v>
       </c>
@@ -19629,7 +19633,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="363" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
         <v>14</v>
       </c>
@@ -19675,7 +19679,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="364" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
         <v>14</v>
       </c>
@@ -19721,7 +19725,7 @@
         <v>45225</v>
       </c>
     </row>
-    <row r="365" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
         <v>14</v>
       </c>
@@ -19959,7 +19963,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="370" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
         <v>14</v>
       </c>
@@ -20007,7 +20011,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="371" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
         <v>14</v>
       </c>
@@ -20055,7 +20059,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="372" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
         <v>14</v>
       </c>
@@ -20101,7 +20105,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="373" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
         <v>14</v>
       </c>
@@ -20147,7 +20151,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="374" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
         <v>14</v>
       </c>
@@ -20193,7 +20197,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="375" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
         <v>14</v>
       </c>
@@ -20239,7 +20243,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="376" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
         <v>14</v>
       </c>
@@ -20285,7 +20289,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="377" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
         <v>14</v>
       </c>
@@ -20331,7 +20335,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="378" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
         <v>14</v>
       </c>
@@ -20379,7 +20383,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="379" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
         <v>14</v>
       </c>
@@ -20427,7 +20431,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="380" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
         <v>14</v>
       </c>
@@ -20473,7 +20477,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="381" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
         <v>14</v>
       </c>
@@ -20519,7 +20523,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="382" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
         <v>14</v>
       </c>
@@ -20565,7 +20569,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="383" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
         <v>14</v>
       </c>
@@ -20611,7 +20615,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="384" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
         <v>14</v>
       </c>
@@ -20657,7 +20661,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="385" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
         <v>14</v>
       </c>
@@ -20703,7 +20707,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="386" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
         <v>14</v>
       </c>
@@ -20751,7 +20755,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="387" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:16" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
         <v>14</v>
       </c>
@@ -20799,7 +20803,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="388" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
         <v>14</v>
       </c>
@@ -20845,7 +20849,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="389" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
         <v>14</v>
       </c>
@@ -20891,7 +20895,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="390" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
         <v>14</v>
       </c>
@@ -20937,7 +20941,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="391" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
         <v>14</v>
       </c>
@@ -20983,7 +20987,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="392" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
         <v>14</v>
       </c>
@@ -21029,7 +21033,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="393" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
         <v>14</v>
       </c>
@@ -21075,7 +21079,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="394" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
         <v>14</v>
       </c>
@@ -21123,7 +21127,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="395" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
         <v>14</v>
       </c>
@@ -21169,7 +21173,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="396" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
         <v>14</v>
       </c>
@@ -21215,7 +21219,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="397" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
         <v>14</v>
       </c>
@@ -21261,7 +21265,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="398" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
         <v>14</v>
       </c>
@@ -21307,7 +21311,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="399" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
         <v>14</v>
       </c>
@@ -21353,7 +21357,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="400" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
         <v>14</v>
       </c>
@@ -21399,7 +21403,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="401" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
         <v>14</v>
       </c>
@@ -21447,7 +21451,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="402" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="2" t="s">
         <v>14</v>
       </c>
@@ -21495,7 +21499,7 @@
         <v>45230</v>
       </c>
     </row>
-    <row r="403" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
         <v>14</v>
       </c>
@@ -21543,7 +21547,7 @@
         <v>45230</v>
       </c>
     </row>
-    <row r="404" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:16" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
         <v>14</v>
       </c>
@@ -21591,7 +21595,7 @@
         <v>45230</v>
       </c>
     </row>
-    <row r="405" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
         <v>14</v>
       </c>
@@ -21639,7 +21643,7 @@
         <v>45230</v>
       </c>
     </row>
-    <row r="406" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
         <v>14</v>
       </c>
@@ -21687,7 +21691,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="407" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
         <v>14</v>
       </c>
@@ -21735,7 +21739,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="408" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
         <v>14</v>
       </c>
@@ -21783,7 +21787,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="409" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
         <v>14</v>
       </c>
@@ -21831,7 +21835,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="410" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" s="2" t="s">
         <v>14</v>
       </c>
@@ -21879,7 +21883,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="411" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" s="2" t="s">
         <v>14</v>
       </c>
@@ -21927,7 +21931,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="412" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" s="2" t="s">
         <v>14</v>
       </c>
@@ -21973,7 +21977,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="413" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
         <v>14</v>
       </c>
@@ -22019,7 +22023,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="414" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
         <v>14</v>
       </c>
@@ -22065,7 +22069,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="415" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
         <v>14</v>
       </c>
@@ -22111,7 +22115,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="416" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" s="2" t="s">
         <v>14</v>
       </c>
@@ -22157,7 +22161,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="417" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" s="2" t="s">
         <v>14</v>
       </c>
@@ -22203,7 +22207,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="418" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" s="2" t="s">
         <v>14</v>
       </c>
@@ -22249,7 +22253,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="419" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
         <v>14</v>
       </c>
@@ -22295,7 +22299,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="420" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
         <v>14</v>
       </c>
@@ -22341,7 +22345,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="421" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
         <v>14</v>
       </c>
@@ -22387,7 +22391,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="422" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
         <v>14</v>
       </c>
@@ -22433,7 +22437,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="423" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
         <v>14</v>
       </c>
@@ -22479,7 +22483,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="424" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
         <v>14</v>
       </c>
@@ -22525,7 +22529,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="425" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
         <v>14</v>
       </c>
@@ -22571,7 +22575,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="426" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" s="2" t="s">
         <v>14</v>
       </c>
@@ -22617,7 +22621,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="427" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
         <v>14</v>
       </c>
@@ -22663,7 +22667,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="428" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" s="2" t="s">
         <v>14</v>
       </c>
@@ -22709,7 +22713,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="429" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" s="2" t="s">
         <v>14</v>
       </c>
@@ -22755,7 +22759,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="430" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" s="2" t="s">
         <v>14</v>
       </c>
@@ -22801,7 +22805,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="431" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" s="2" t="s">
         <v>14</v>
       </c>
@@ -22847,7 +22851,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="432" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" s="2" t="s">
         <v>14</v>
       </c>
@@ -22893,7 +22897,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="433" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" s="2" t="s">
         <v>14</v>
       </c>
@@ -22939,7 +22943,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="434" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" s="2" t="s">
         <v>14</v>
       </c>
@@ -22985,7 +22989,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="435" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" s="2" t="s">
         <v>14</v>
       </c>
@@ -23031,7 +23035,7 @@
         <v>45232</v>
       </c>
     </row>
-    <row r="436" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" s="2" t="s">
         <v>14</v>
       </c>
@@ -23079,7 +23083,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="437" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" s="2" t="s">
         <v>14</v>
       </c>
@@ -23127,7 +23131,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="438" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" s="2" t="s">
         <v>14</v>
       </c>
@@ -23175,7 +23179,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="439" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" s="2" t="s">
         <v>14</v>
       </c>
@@ -23223,7 +23227,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="440" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
         <v>14</v>
       </c>
@@ -23271,7 +23275,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="441" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
         <v>14</v>
       </c>
@@ -23319,7 +23323,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="442" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
         <v>14</v>
       </c>
@@ -23365,7 +23369,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="443" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" s="2" t="s">
         <v>14</v>
       </c>
@@ -23413,7 +23417,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="444" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" s="2" t="s">
         <v>14</v>
       </c>
@@ -23461,7 +23465,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="445" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" s="2" t="s">
         <v>14</v>
       </c>
@@ -23509,7 +23513,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="446" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" s="2" t="s">
         <v>14</v>
       </c>
@@ -23555,7 +23559,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="447" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
         <v>14</v>
       </c>
@@ -23603,7 +23607,7 @@
         <v>45236</v>
       </c>
     </row>
-    <row r="448" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
         <v>14</v>
       </c>
@@ -23651,7 +23655,7 @@
         <v>45236</v>
       </c>
     </row>
-    <row r="449" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" s="2" t="s">
         <v>14</v>
       </c>
@@ -23699,7 +23703,7 @@
         <v>45236</v>
       </c>
     </row>
-    <row r="450" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450" s="2" t="s">
         <v>14</v>
       </c>
@@ -23747,7 +23751,7 @@
         <v>45236</v>
       </c>
     </row>
-    <row r="451" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451" s="2" t="s">
         <v>14</v>
       </c>
@@ -23795,7 +23799,7 @@
         <v>45236</v>
       </c>
     </row>
-    <row r="452" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" s="2" t="s">
         <v>14</v>
       </c>
@@ -23843,7 +23847,7 @@
         <v>45236</v>
       </c>
     </row>
-    <row r="453" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" s="2" t="s">
         <v>14</v>
       </c>
@@ -23891,7 +23895,7 @@
         <v>45236</v>
       </c>
     </row>
-    <row r="454" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" s="2" t="s">
         <v>14</v>
       </c>
@@ -23939,7 +23943,7 @@
         <v>45237</v>
       </c>
     </row>
-    <row r="455" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455" s="2" t="s">
         <v>14</v>
       </c>
@@ -23987,7 +23991,7 @@
         <v>45237</v>
       </c>
     </row>
-    <row r="456" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" s="2" t="s">
         <v>14</v>
       </c>
@@ -24035,7 +24039,7 @@
         <v>45237</v>
       </c>
     </row>
-    <row r="457" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457" s="2" t="s">
         <v>14</v>
       </c>
@@ -24083,7 +24087,7 @@
         <v>45237</v>
       </c>
     </row>
-    <row r="458" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:16" ht="23.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" s="2" t="s">
         <v>14</v>
       </c>
@@ -24131,7 +24135,7 @@
         <v>45237</v>
       </c>
     </row>
-    <row r="459" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
         <v>14</v>
       </c>
@@ -24179,7 +24183,7 @@
         <v>45238</v>
       </c>
     </row>
-    <row r="460" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
         <v>14</v>
       </c>
@@ -24227,7 +24231,7 @@
         <v>45238</v>
       </c>
     </row>
-    <row r="461" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
         <v>14</v>
       </c>
@@ -24275,7 +24279,7 @@
         <v>45238</v>
       </c>
     </row>
-    <row r="462" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
         <v>14</v>
       </c>
@@ -24323,7 +24327,7 @@
         <v>45238</v>
       </c>
     </row>
-    <row r="463" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
         <v>14</v>
       </c>
@@ -24371,7 +24375,7 @@
         <v>45238</v>
       </c>
     </row>
-    <row r="464" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
         <v>14</v>
       </c>
@@ -24419,7 +24423,7 @@
         <v>45238</v>
       </c>
     </row>
-    <row r="465" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
         <v>14</v>
       </c>
@@ -24465,7 +24469,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="466" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
         <v>14</v>
       </c>
@@ -24511,7 +24515,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="467" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
         <v>14</v>
       </c>
@@ -24557,7 +24561,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="468" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" s="2" t="s">
         <v>14</v>
       </c>
@@ -24603,7 +24607,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="469" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469" s="2" t="s">
         <v>14</v>
       </c>
@@ -24649,7 +24653,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="470" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" s="2" t="s">
         <v>14</v>
       </c>
@@ -24695,7 +24699,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="471" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" s="2" t="s">
         <v>14</v>
       </c>
@@ -24743,7 +24747,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="472" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472" s="2" t="s">
         <v>14</v>
       </c>
@@ -24789,7 +24793,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="473" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473" s="2" t="s">
         <v>14</v>
       </c>
@@ -24835,7 +24839,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="474" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474" s="2" t="s">
         <v>14</v>
       </c>
@@ -24881,7 +24885,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="475" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
         <v>14</v>
       </c>
@@ -24927,7 +24931,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="476" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476" s="2" t="s">
         <v>14</v>
       </c>
@@ -24973,7 +24977,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="477" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477" s="2" t="s">
         <v>14</v>
       </c>
@@ -25019,7 +25023,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="478" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478" s="2" t="s">
         <v>14</v>
       </c>
@@ -25065,7 +25069,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="479" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479" s="2" t="s">
         <v>14</v>
       </c>
@@ -25111,7 +25115,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="480" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480" s="2" t="s">
         <v>14</v>
       </c>
@@ -25157,7 +25161,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="481" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481" s="2" t="s">
         <v>14</v>
       </c>
@@ -25203,7 +25207,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="482" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A482" s="2" t="s">
         <v>14</v>
       </c>
@@ -25249,7 +25253,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="483" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483" s="2" t="s">
         <v>14</v>
       </c>
@@ -25295,7 +25299,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="484" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484" s="2" t="s">
         <v>14</v>
       </c>
@@ -25343,7 +25347,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="485" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485" s="2" t="s">
         <v>14</v>
       </c>
@@ -25389,7 +25393,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="486" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" s="2" t="s">
         <v>14</v>
       </c>
@@ -25435,7 +25439,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="487" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487" s="2" t="s">
         <v>14</v>
       </c>
@@ -25481,7 +25485,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="488" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
         <v>14</v>
       </c>
@@ -25527,7 +25531,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="489" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
         <v>14</v>
       </c>
@@ -25573,7 +25577,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="490" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
         <v>14</v>
       </c>
@@ -25619,7 +25623,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="491" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491" s="2" t="s">
         <v>14</v>
       </c>
@@ -25667,7 +25671,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="492" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" s="2" t="s">
         <v>14</v>
       </c>
@@ -25715,7 +25719,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="493" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A493" s="2" t="s">
         <v>14</v>
       </c>
@@ -25763,7 +25767,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="494" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494" s="2" t="s">
         <v>14</v>
       </c>
@@ -25811,7 +25815,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="495" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A495" s="2" t="s">
         <v>14</v>
       </c>
@@ -25859,7 +25863,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="496" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496" s="2" t="s">
         <v>14</v>
       </c>
@@ -25907,7 +25911,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="497" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A497" s="2" t="s">
         <v>14</v>
       </c>
@@ -25955,7 +25959,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="498" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" s="2" t="s">
         <v>14</v>
       </c>
@@ -26003,7 +26007,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="499" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:16" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A499" s="2" t="s">
         <v>14</v>
       </c>
@@ -26051,7 +26055,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="500" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:16" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A500" s="2" t="s">
         <v>14</v>
       </c>
@@ -26099,7 +26103,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="501" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:16" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A501" s="2" t="s">
         <v>14</v>
       </c>
@@ -48564,7 +48568,19 @@
       <c r="D7973" s="141"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N501" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A1:N501" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <filterColumn colId="4">
+      <filters>
+        <dateGroupItem year="2024" month="6" day="27" dateTimeGrouping="day"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters>
+        <filter val="A01-A08"/>
+        <filter val="ALL"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N501">
     <sortCondition ref="F2:F501"/>
   </sortState>
@@ -48578,12 +48594,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -48766,15 +48779,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFC73EDA-6B2F-4B5B-858E-6AD4B6E182A8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{836137F5-2A5A-4F0D-935E-C8DB69844C45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -48799,10 +48816,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{836137F5-2A5A-4F0D-935E-C8DB69844C45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFC73EDA-6B2F-4B5B-858E-6AD4B6E182A8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>